<commit_message>
Changes to be committed:
modified:   Paris-web-2019-tester-pour-les-nuls.pptx

new file:   atelier/checklists-atelier.zip

modified:   atelier/corrige/Portail-tests-CONCEPTEUR.xlsx

modified:   atelier/html/js/vendor/script.js

modified:   atelier/html/notes-de-frais.html

modified:   atelier/html/portail-content.html

modified:   atelier/html/portail.html

modified:   atelier/html/transfert-fichier.html
</commit_message>
<xml_diff>
--- a/atelier/corrige/Portail-tests-CONCEPTEUR.xlsx
+++ b/atelier/corrige/Portail-tests-CONCEPTEUR.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="13605" yWindow="105" windowWidth="15105" windowHeight="12750"/>
+    <workbookView xWindow="13605" yWindow="105" windowWidth="15105" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -688,7 +688,7 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">structure à améliorer (menu, différentes parties du contenu…).
-Par exemple le menu des catégorie de news n'est pas correctement identifiable (difficulté pour des mal-voyant de comprendre ce composant comme un menu, difficulté pour d'enpercevoir les limites). Les liens soulignés dans les blocs ne sont pas pertinents, et rendent difficile la lecture). Dans ce contexte la notion de liens est compréhensible sans le souligné.
+Par exemple le menu des catégorie de news n'est pas correctement identifiable (difficulté pour des mal-voyant de comprendre ce composant comme un menu, difficulté pour d'enpercevoir les limites). Les liens soulignés dans les blocs ne sont pas pertinents, et rendent difficile la lecture). Dans ce contexte la notion de liens est compréhensible sans le souligné. Il existe 2 titrues "derneirs ajouts" qui ne concerne pas les mêmes types contenus.
 </t>
     </r>
     <r>
@@ -710,7 +710,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>ajouter à minima un repère visuel (exemple une bordure), pour permettre à tous les utilisateurs d'identifier facilement ce regroupement d'items, et ses limites (garder en tête que certains utilisateurs ne voient pas la totalité de l'écran).</t>
+      <t>ajouter à minima un repère visuel (exemple une bordure), pour permettre à tous les utilisateurs d'identifier facilement ce regroupement d'items, et ses limites (garder en tête que certains utilisateurs ne voient pas la totalité de l'écran). Différencier les deux titres "Derniers ajouts", en précisant de quoi il s'agit.</t>
     </r>
   </si>
 </sst>
@@ -1288,7 +1288,7 @@
   <dimension ref="A1:C185"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1431,7 +1431,7 @@
       <c r="B17" s="7"/>
       <c r="C17" s="8"/>
     </row>
-    <row r="18" spans="1:3" ht="165" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="195" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>18</v>
       </c>

</xml_diff>